<commit_message>
Added method todense() for sparse csr matrix.
</commit_message>
<xml_diff>
--- a/doc/ImplementationStatus.xlsx
+++ b/doc/ImplementationStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\zkj327\coding\otilib-master\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{962D7AB3-BD78-4F43-8EA2-933B53ECAAFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4403566E-D7BA-4B5C-91B5-99BB0ED6144A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13830" activeTab="3"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I28" sqref="I27:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.21875" defaultRowHeight="15.95"/>

</xml_diff>